<commit_message>
new features + modifying
app.py: we added new imports and added new functionality for  new websites.

added france.py
added norway.py
added sweden.py

search.html: added 3 new options for new websites.
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,340 +453,884 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mitic, Zoran</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Chörbli 2, 6020 Emmenbrücke LU</t>
-        </is>
-      </c>
+          <t>Aleksandar Mitic</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>41412601952</t>
+          <t>['465 08 335']</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mitic, Aleksandar</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Zelgli 4, 8413 Neftenbach ZH</t>
-        </is>
-      </c>
+          <t>Aleksandra Mitic</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>N/A</t>
+          <t>['485 02 750']</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mitic, Berislav</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Thurblick 8, 9246 Niederbüren SG</t>
-        </is>
-      </c>
+          <t>Aleksandra Nikolic-Mitic</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>41719251112</t>
+          <t>['981 79 933']</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Mitic, Danijela</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Sangenstrasse 6, 8570 Weinfelden TG</t>
-        </is>
-      </c>
+          <t>Alexander Mitic</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>41716229370</t>
+          <t>['484 29 852']</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Mitic, Dragan</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Dorf 27, 6166 Hasle LU</t>
-        </is>
-      </c>
+          <t>Ana Mitic Radojicic</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>41414800425</t>
+          <t>['463 48 451']</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Mitic, Dragoljub (-Stanojevic)</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Listrigstrasse 9, 6020 Emmenbrücke LU</t>
-        </is>
-      </c>
+          <t>Bogdan Mitic</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>41412810206</t>
+          <t>['942 87 134']</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Mitic, Goran</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Sagenbachmatt 2, 6280 Hochdorf LU</t>
-        </is>
-      </c>
+          <t>Bratislav Mitic</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>41419103318</t>
+          <t>['462 40 952']</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mitic, Hranislav</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Quellhölzlistrasse 1, 5032 Aarau Rohr AG</t>
-        </is>
-      </c>
+          <t>Daliborka Mitic</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>41628223590</t>
+          <t>['471 44 614']</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Mitic, Isailo</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Avenue Edouard-Dapples 36, 1006 Lausanne</t>
-        </is>
-      </c>
+          <t>Dragan Mitic</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>41216173159</t>
+          <t>['412 73 436']</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mitic, Jasmina</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Längweiherstrasse 14, 6014 Luzern</t>
-        </is>
-      </c>
+          <t>Ivan Mitic</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>41412502623</t>
+          <t>['902 41 991']</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Mitic, Marta</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Burgstrasse 7, 8604 Volketswil ZH</t>
-        </is>
-      </c>
+          <t>Ivan Mitic</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>41438101866</t>
+          <t>['939 63 980']</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Mitic, Milana</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Willestrasse 14, 3400 Burgdorf BE</t>
-        </is>
-      </c>
+          <t>Julijana Mitic</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>41344226219</t>
+          <t>['485 03 503']</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Mitic, Momcilo</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Rudishaldenstrasse 4, 8800 Thalwil ZH</t>
-        </is>
-      </c>
+          <t>Katarina Mitic</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>41447210830</t>
+          <t>['908 36 575']</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Mitic, Olga</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Im Grüntal 15, 8405 Winterthur</t>
-        </is>
-      </c>
+          <t>Maria Mitic</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>41448219574</t>
+          <t>['986 83 060']</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Mitic, Radmila</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Rieven 18, 7013 Domat/Ems GR</t>
-        </is>
-      </c>
+          <t>Milena Mitic</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>41816333205</t>
+          <t>['463 63 323']</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Mitic, Slavisa</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Feldlistrasse 17, 9000 St. Gallen</t>
-        </is>
-      </c>
+          <t>Milena Mitic</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>41712786132</t>
+          <t>['463 63 323']</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Mitic, Stojan</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Bahnhofstrasse 27, 6244 Nebikon LU</t>
-        </is>
-      </c>
+          <t>Milorad Mitic</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>41787512766</t>
+          <t>['37 01 61 03']</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Mitic, Svetlana</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Blümlisalpstrasse 12, 3076 Worb BE</t>
-        </is>
-      </c>
+          <t>Nikola Mitic</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>41318321971</t>
+          <t>['477 47 288']</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Mitic, Tamara</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Furkastrasse 89, 3984 Fiesch VS</t>
-        </is>
-      </c>
+          <t>Svetlana Mitic</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>41279732285</t>
+          <t>['415 67 301']</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Mitic, Tatjana</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Route de Bressaucourt 61A, 2900 Porrentruy JU</t>
-        </is>
-      </c>
+          <t>Svetlana Mitic</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
-          <t>41324668705</t>
+          <t>['915 20 281']</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Vladica Mitic</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>['925 67 659']</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Vukasin Mitic</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>['967 30 433']</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Zeljko Mitic</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>['944 92 763']</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Adrian Matic</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr"/>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>['918 85 485']</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Aleksandar Matic</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr"/>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>['930 66 138']</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Ana Matic</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr"/>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>['944 78 280']</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Andrea Matic</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>['465 19 401']</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Anela Matic</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>['917 18 481']</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Anne Matic</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>['463 03 924']</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Boris Matic</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr"/>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>['465 73 638']</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Borislav Matic</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>['75 51 14 14']</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Daniela Matic</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>['402 89 185']</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Danijela Matic</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>['484 22 097', '473 63 445']</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>David Florian Matic</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>['907 12 374']</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Dorian Matic</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>['452 18 307']</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Efren Matic Buenaventura</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>['907 43 114']</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Gordana Matic</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>['958 03 962']</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Hanna Matic</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>['475 03 346']</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Hanna Matic</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>['950 06 047']</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Ira Matic-Krstic</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>['408 90 962']</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Iren Matic</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr"/>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>['51 54 35 38', '984 42 553']</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Isabella Matic</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>['949 82 541']</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Ivo Matic</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>['967 58 885']</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Ivona Matic-Krstic</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>['980 47 345']</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Josip Matic</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr"/>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>['407 20 849']</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Josipa Matic</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr"/>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>['904 75 585']</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Katarina Matic</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>['458 30 664']</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Katinka Matic</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>['994 80 123']</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Maria Matic</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr"/>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>['981 04 878']</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Marko Matic</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr"/>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>['477 24 999']</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Martina Nezic-Matic</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr"/>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>['481 06 301']</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Matic Gajsek</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr"/>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>['922 89 871']</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Mato Matic</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>['970 36 686']</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Milan Matic</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr"/>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>['925 66 767']</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Nebojsa Matic</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>['922 20 523']</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Nena Matic</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>['413 11 544']</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Petra Matic</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr"/>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>['929 86 645']</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Sasa Matic</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr"/>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>['463 48 635']</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Stanko Matic</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr"/>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>['939 20 293']</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Strahinj Matic</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr"/>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>['929 86 642']</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Tatjana Maria Siemer</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr"/>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>['464 14 692']</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Teo Matic</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>['412 13 319']</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Tihomir Frane Matic</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>['939 68 869']</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Vladimir Matic</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr"/>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>['406 25 848']</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Vladimir Matic</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr"/>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>['480 50 788']</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Vuk Matic</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr"/>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>['929 86 643']</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Anja Mitikj</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr"/>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>['452 96 234']</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Milosh Mitikj</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr"/>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>['415 47 599']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
all bugs are fixed on belgium,germany,italia and sweden. Everything is ready for review.
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,799 +453,527 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Mitic Bozidar</t>
+          <t>IGOR JOVANOVIC</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Triester Str 158, 1230 Wien</t>
+          <t>Rue du Commerce 51, 4100 Seraing</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>+43 699 10781393</t>
+          <t>3243396154</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mitic Verica</t>
+          <t>Verica Jovanovic</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Borschkeg 12, 1090 Wien</t>
+          <t>Paardenmarktstraat 129, 3080 Tervuren</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>+43 676 9441589</t>
+          <t>3227680286</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mitic Verica</t>
+          <t>Jovanovic Dragica</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Urschenböckg 8, 1110 Wien</t>
+          <t>Rue Général Henry 134, 1040 Etterbeek</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>+43 676 6365021</t>
+          <t>3223100295</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Mitic Vodosav</t>
+          <t>Jovanovic Draga</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Josef-Gruber-G 2, 5020 Salzburg</t>
+          <t>Akkerstraat 23, 3680 Neeroeteren (Maaseik)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>+43 662 821587</t>
+          <t>3289215951</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Mitic Ljulisa</t>
+          <t>Nikola Jovanovic</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Krenng 34, 8010 Graz</t>
+          <t>Drève des Equipages 16, 1170 Watermael-Boitsfort</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>+43 316 849451</t>
+          <t>3226602204</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Mitic Zivislav</t>
+          <t>Joey Jovanovic</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Hütteldorfer Str 117, 1140 Wien</t>
+          <t>Rue des Etangs Noirs 89, 1080 Molenbeek-Saint-Jean</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>+43 1 9714069</t>
+          <t>3226404787</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Mitic Mirjana</t>
+          <t>DRAGANA JOVANOVIC</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Arnethg 107, 1160 Wien</t>
+          <t>Rue Péterson 7, 5580 Jemelle (Rochefort)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>+43 1 4086421</t>
+          <t>3284730307</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mitic Zivorat</t>
+          <t>SVETLANA JOVANOVIC</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Nauseag 14, 1160 Wien</t>
+          <t>Rue du Warmonceau 33, 6061 Montignies-sur-Sambre (Charleroi)</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>+43 1 9234456</t>
+          <t>3271120443</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Mitic Nebojsa</t>
+          <t>SIBIN JOVANOVIC</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Hütteldorfer Str 117, 1140 Wien</t>
+          <t>Kapellenboslaan 35, 2830 Willebroek</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>+43 699 19714062</t>
+          <t>3234374396</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mitic Zivadin</t>
+          <t>DAVID JOVANOVIC</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Münchendorfer Str 12-14, 2353 Guntramsdorf</t>
+          <t>Rue de Montegnée 2, 4101 Jemeppe-sur-Meuse (Seraing)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>+43 2236 56738</t>
+          <t>3243911905</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Mitic Srdjan</t>
+          <t>Jika Jovanovic</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Hellbrunner Allee 59, 5020 Salzburg</t>
+          <t>Petite Rue du Moulin 26, 1070 Anderlecht</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>+43 664 3432157</t>
+          <t>3226444124</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Mitic Olga</t>
+          <t>RENATE JOVANOVIC</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ettenreichg 16, 1100 Wien</t>
+          <t>Domaine des Maraîchers 68, 7390 Wasmuel (Quaregnon)</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>+43 676 7043271</t>
+          <t>3265641298</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Mitic Sladjan, DI</t>
+          <t>ANITA JOVANOVIC</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Viktorg 17, 1040 Wien</t>
+          <t>KERKENDIJK 19, 2000 ANTWERPEN</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>+43 1 9136797</t>
+          <t>3234370683</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Mitic Daniela</t>
+          <t>Tycha Jovanovic</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Hetzendorfer Str 103, Stg 3, 1120 Wien</t>
+          <t>Rue du Fond 8, 4920 Sougné-Remouchamps (Aywaille)</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>+43 1 9247052</t>
+          <t>3242431388</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Mitic Zvonko</t>
+          <t>MILAN JOVANOVIC</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Sauterg 15, 1170 Wien</t>
+          <t>Rue Jean Noté 42, 1070 Anderlecht</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>+43 1 9249096</t>
+          <t>3225234241</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Mitic Sladjana</t>
+          <t>LAORA JOVANOVIC</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Nikelsdorf, Dr.Schaumberger Weg 100, 9711 Paternion</t>
+          <t>Rue Arthur Decoux 54, 6020 Dampremy (Charleroi)</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>+43 676 9560722</t>
+          <t>3271575700</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Mitic Danijela</t>
+          <t>Jovanovic Branko</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Redtenbacherg 48, 1160 Wien</t>
+          <t>Avenue des Sorbiers 11, 1330 Rixensart</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>+43 650 8311236</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Mitic Suvad</t>
+          <t>DZULISTANA JOVANOVIC</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Innerkoflerstr 1A, 6020 Innsbruck</t>
+          <t>Rue Edmond Leburton 14, 6200 Châtelineau (Châtelet)</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>+43 650 4280040</t>
+          <t>3271972091</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Mitic Ana</t>
+          <t>Dragana Jovanovic</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Wichtelg 9, 1160 Wien</t>
+          <t>Rue des Alouettes 32, 7100 La Louvière</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>+43 699 12900463</t>
+          <t>3264222958</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Mitic Renate</t>
+          <t>DARKO JOVANOVIC</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Pirka, Packer Str 92A, 8054 Seiersberg-Pirka</t>
+          <t>KESSELDAALLAAN 8, 3010 KESSEL-LO</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>+43 316 289486</t>
+          <t>3216427363</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Mitic Dejan</t>
+          <t>Draga Jovanovic</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Inzersdorfer Str 74 Stg 1, 1100 Wien</t>
+          <t>Dascottelei 55/401, 2100 Deurne (Anvers)</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>+43 1 9203186</t>
+          <t>3233211267</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Mitic Slavisa</t>
+          <t>SANJA JOVANOVIC</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Gießaufg 23, 1050 Wien</t>
+          <t>Kampioenstraat 26, 2020 Anvers</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>+43 650 9129277</t>
+          <t>3232764929</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Mitic Milovan</t>
+          <t>Srdan Jovanovic</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Wöllersdorfer Str 8, 2700 Wiener Neustadt</t>
+          <t>Daliastraat 12, 2580 Putte</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>+43 650 2911150</t>
+          <t>3215760287</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Mitic Nenad</t>
+          <t>DOBRICA JOVANOVIC</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Engerthstr 149, 1020 Wien</t>
+          <t>Rue des Pâquerettes 52, 7160 Chapelle-lez-Herlaimont</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>+43 699 19781806</t>
+          <t>3264382648</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Mitic Rosica</t>
+          <t>DARKO JOVANOVIC</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Rötzerg 44, 1170 Wien</t>
+          <t>Kesseldallaan 8, 3010 Kessel-Lo (Louvain)</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>+43 660 1247055</t>
+          <t>3216750744</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Mitic Ljubišsav</t>
+          <t>Marija Jovanovic</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Krenng 34, 8010 Graz</t>
+          <t>Oranjestraat 31 R, 2060 Anvers</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>+43 664 3251105</t>
+          <t>3232319317</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Mitic Svetlana</t>
+          <t>Isnija Jovanovic</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Inzersdorfer Str 74 Stg 1, 1100 Wien</t>
+          <t>Rue de l'Ourthe 31, 1080 Molenbeek-Saint-Jean</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>+43 699 11364620</t>
+          <t>3226443721</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Mitic Dobrivoje</t>
+          <t>Jelica Jovanovic</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Fürbergstr 4, 5020 Salzburg</t>
+          <t>Laurian-Moris-Straße 17, 4780 Saint-Vith</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>+43 664 2332335</t>
+          <t>3280685676</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Mitic Dobrinka</t>
+          <t>Samantha Jovanovic</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Castellezg 8, 1020 Wien</t>
+          <t>Boulevard Joseph Tirou 10 00O7, 6000 Charleroi</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>+43 664 1246862</t>
+          <t>3271819213</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Mitic Jelena</t>
+          <t>Dusko Jovanovic</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Feldkreuzweg 25, 6800 Feldkirch</t>
+          <t>Rue Willems 45/5, 1210 Saint-Josse-ten-Noode</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>+43 650 9261058</t>
+          <t>3223301843</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Mitic Nenad</t>
+          <t>Milorad Jovanovic</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Penzinger Str 33-37 Stg 6, 1140 Wien</t>
+          <t>Rue de l'Harmonie 7 b007, 1000 Bruxelles</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>+43 1 9165578</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Mitic Pavle</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Siccardsburgg 37, 1100 Wien</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>+43 664 5644251</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Mitic Mirjana</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Breitenfurter Str 241 Stg 1, 1230 Wien</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>+43 664 4459505</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Mitic Slavisa</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Vivariumstr 6 Stg 1, 1020 Wien</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>+43 1 7295027</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Mitic Nevenka</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>Gutenhoferstr 13, 2325 Himberg</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>+43 676 7903461</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Mitic Zivko</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>Wittau, Getreideweg 9, 2301 Groß-Enzersdorf</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>+43 660 3825656</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Mitic Darko</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Eisenreichs, 27, 3834 Pfaffenschlag bei Waidhofen a.d.Thaya</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>+43 650 6854515</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Mitic Branka</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Inzersdorfer Str 111, 1100 Wien</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>+43 699 10339507</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Mitic Vladica</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Schererstr 12B, 4663 Laakirchen</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>+43 664 2020543</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Mitic Adrijana</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Auwiesenstr 27, 5161 Elixhausen</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>+43 664 5160539</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Mitic Barbara</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Schwalbeng 31, 5111 Bürmoos</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>+43 650 2647616</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Mitic Mirsad</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Rudolf-Zeller-G 58-60 Stg 8, 1230 Wien</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>+43 690 10351261</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Mitic Zivorad</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>Thimigg 19, 1180 Wien</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>+43 1 9201198</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Mitic Darko</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>Hermanng 4, 1070 Wien</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>+43 1 9574187</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Mitic Majda</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Rudolf-Zeller-G 58-60 Stg 8, 1230 Wien</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>+43 690 10441307</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>Mitic Slobodan</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Haberlg 64, 1160 Wien</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>+43 1 9900921</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Mitic Renate</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Seiersberg, Anzengruberg 7, 8055 Seiersberg-Pirka</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>+43 316 241326</t>
+          <t>N/A</t>
         </is>
       </c>
     </row>

</xml_diff>